<commit_message>
Minors changes and implementations before beta testing
</commit_message>
<xml_diff>
--- a/Stats 2.xlsx
+++ b/Stats 2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Software Development\SAT Project\sat-development-Angus408\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{15BBE262-DE48-4238-B472-D5BF458CE0E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AB2E3A5-7132-4019-BEFE-36952622947E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{37EEF028-F0DD-4D8B-BCAA-9B785BCAAE0C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="27">
   <si>
     <t>Craigieburn 3s</t>
   </si>
@@ -111,6 +111,12 @@
   </si>
   <si>
     <t>Tristyn</t>
+  </si>
+  <si>
+    <t>Altona 5s</t>
+  </si>
+  <si>
+    <t>Lucas</t>
   </si>
 </sst>
 </file>
@@ -132,7 +138,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -169,6 +175,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFF2CC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -197,7 +209,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -215,6 +227,9 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -551,15 +566,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A70EC3EB-5950-48A1-AFCB-F6AFC1DA3D6C}">
-  <dimension ref="A1:P10"/>
+  <dimension ref="A1:S24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:16" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:19" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -609,7 +624,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
         <v>16</v>
       </c>
@@ -659,7 +674,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
         <v>17</v>
       </c>
@@ -709,7 +724,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="2" t="s">
         <v>18</v>
       </c>
@@ -759,7 +774,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="2" t="s">
         <v>19</v>
       </c>
@@ -809,7 +824,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="2" t="s">
         <v>20</v>
       </c>
@@ -859,7 +874,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="2" t="s">
         <v>21</v>
       </c>
@@ -909,7 +924,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="2" t="s">
         <v>22</v>
       </c>
@@ -959,7 +974,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="2" t="s">
         <v>23</v>
       </c>
@@ -1009,7 +1024,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="2" t="s">
         <v>24</v>
       </c>
@@ -1056,6 +1071,557 @@
         <v>1</v>
       </c>
       <c r="P10" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="14" spans="1:19" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D14" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="M14" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N14" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="O14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="P14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="R14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="S14" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D15" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E15" s="3">
+        <v>2</v>
+      </c>
+      <c r="F15" s="3">
+        <v>0</v>
+      </c>
+      <c r="G15" s="3">
+        <v>0</v>
+      </c>
+      <c r="H15" s="3">
+        <v>0</v>
+      </c>
+      <c r="I15" s="4">
+        <v>2</v>
+      </c>
+      <c r="J15" s="4">
+        <v>0</v>
+      </c>
+      <c r="K15" s="3">
+        <v>0</v>
+      </c>
+      <c r="L15" s="3">
+        <v>0</v>
+      </c>
+      <c r="M15" s="5">
+        <v>3</v>
+      </c>
+      <c r="N15" s="5">
+        <v>2</v>
+      </c>
+      <c r="O15" s="3">
+        <v>0</v>
+      </c>
+      <c r="P15" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="3">
+        <v>0</v>
+      </c>
+      <c r="R15" s="4">
+        <v>1</v>
+      </c>
+      <c r="S15" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D16" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" s="3">
+        <v>2</v>
+      </c>
+      <c r="F16" s="3">
+        <v>0</v>
+      </c>
+      <c r="G16" s="3">
+        <v>1</v>
+      </c>
+      <c r="H16" s="3">
+        <v>0</v>
+      </c>
+      <c r="I16" s="4">
+        <v>3</v>
+      </c>
+      <c r="J16" s="4">
+        <v>0</v>
+      </c>
+      <c r="K16" s="3">
+        <v>0</v>
+      </c>
+      <c r="L16" s="3">
+        <v>0</v>
+      </c>
+      <c r="M16" s="3">
+        <v>0</v>
+      </c>
+      <c r="N16" s="3">
+        <v>0</v>
+      </c>
+      <c r="O16" s="3">
+        <v>0</v>
+      </c>
+      <c r="P16" s="5">
+        <v>2</v>
+      </c>
+      <c r="Q16" s="3">
+        <v>0</v>
+      </c>
+      <c r="R16" s="4">
+        <v>1</v>
+      </c>
+      <c r="S16" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="4:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D17" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E17" s="3">
+        <v>6</v>
+      </c>
+      <c r="F17" s="3">
+        <v>1</v>
+      </c>
+      <c r="G17" s="3">
+        <v>2</v>
+      </c>
+      <c r="H17" s="3">
+        <v>0</v>
+      </c>
+      <c r="I17" s="4">
+        <v>8</v>
+      </c>
+      <c r="J17" s="4">
+        <v>1</v>
+      </c>
+      <c r="K17" s="4">
+        <v>2</v>
+      </c>
+      <c r="L17" s="4">
+        <v>0</v>
+      </c>
+      <c r="M17" s="3">
+        <v>0</v>
+      </c>
+      <c r="N17" s="3">
+        <v>1</v>
+      </c>
+      <c r="O17" s="3">
+        <v>1</v>
+      </c>
+      <c r="P17" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="3">
+        <v>0</v>
+      </c>
+      <c r="R17" s="4">
+        <v>3</v>
+      </c>
+      <c r="S17" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="4:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D18" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E18" s="3">
+        <v>5</v>
+      </c>
+      <c r="F18" s="3">
+        <v>3</v>
+      </c>
+      <c r="G18" s="3">
+        <v>1</v>
+      </c>
+      <c r="H18" s="3">
+        <v>1</v>
+      </c>
+      <c r="I18" s="5">
+        <v>6</v>
+      </c>
+      <c r="J18" s="5">
+        <v>4</v>
+      </c>
+      <c r="K18" s="3">
+        <v>0</v>
+      </c>
+      <c r="L18" s="3">
+        <v>0</v>
+      </c>
+      <c r="M18" s="3">
+        <v>0</v>
+      </c>
+      <c r="N18" s="3">
+        <v>1</v>
+      </c>
+      <c r="O18" s="5">
+        <v>2</v>
+      </c>
+      <c r="P18" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q18" s="3">
+        <v>0</v>
+      </c>
+      <c r="R18" s="4">
+        <v>3</v>
+      </c>
+      <c r="S18" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="4:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D19" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E19" s="3">
+        <v>3</v>
+      </c>
+      <c r="F19" s="3">
+        <v>0</v>
+      </c>
+      <c r="G19" s="3">
+        <v>1</v>
+      </c>
+      <c r="H19" s="3">
+        <v>1</v>
+      </c>
+      <c r="I19" s="4">
+        <v>4</v>
+      </c>
+      <c r="J19" s="4">
+        <v>1</v>
+      </c>
+      <c r="K19" s="3">
+        <v>0</v>
+      </c>
+      <c r="L19" s="3">
+        <v>0</v>
+      </c>
+      <c r="M19" s="3">
+        <v>0</v>
+      </c>
+      <c r="N19" s="3">
+        <v>0</v>
+      </c>
+      <c r="O19" s="3">
+        <v>1</v>
+      </c>
+      <c r="P19" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q19" s="3">
+        <v>0</v>
+      </c>
+      <c r="R19" s="4">
+        <v>2</v>
+      </c>
+      <c r="S19" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="4:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D20" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E20" s="3">
+        <v>6</v>
+      </c>
+      <c r="F20" s="3">
+        <v>2</v>
+      </c>
+      <c r="G20" s="3">
+        <v>0</v>
+      </c>
+      <c r="H20" s="3">
+        <v>0</v>
+      </c>
+      <c r="I20" s="7">
+        <v>6</v>
+      </c>
+      <c r="J20" s="7">
+        <v>2</v>
+      </c>
+      <c r="K20" s="3">
+        <v>0</v>
+      </c>
+      <c r="L20" s="3">
+        <v>0</v>
+      </c>
+      <c r="M20" s="5">
+        <v>3</v>
+      </c>
+      <c r="N20" s="5">
+        <v>2</v>
+      </c>
+      <c r="O20" s="3">
+        <v>0</v>
+      </c>
+      <c r="P20" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q20" s="3">
+        <v>1</v>
+      </c>
+      <c r="R20" s="4">
+        <v>1</v>
+      </c>
+      <c r="S20" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="4:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D21" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E21" s="3">
+        <v>6</v>
+      </c>
+      <c r="F21" s="3">
+        <v>1</v>
+      </c>
+      <c r="G21" s="3">
+        <v>0</v>
+      </c>
+      <c r="H21" s="3">
+        <v>0</v>
+      </c>
+      <c r="I21" s="4">
+        <v>6</v>
+      </c>
+      <c r="J21" s="4">
+        <v>1</v>
+      </c>
+      <c r="K21" s="5">
+        <v>2</v>
+      </c>
+      <c r="L21" s="5">
+        <v>1</v>
+      </c>
+      <c r="M21" s="5">
+        <v>2</v>
+      </c>
+      <c r="N21" s="3">
+        <v>1</v>
+      </c>
+      <c r="O21" s="3">
+        <v>0</v>
+      </c>
+      <c r="P21" s="5">
+        <v>2</v>
+      </c>
+      <c r="Q21" s="3">
+        <v>1</v>
+      </c>
+      <c r="R21" s="4">
+        <v>4</v>
+      </c>
+      <c r="S21" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="4:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D22" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E22" s="3">
+        <v>9</v>
+      </c>
+      <c r="F22" s="3">
+        <v>2</v>
+      </c>
+      <c r="G22" s="3">
+        <v>0</v>
+      </c>
+      <c r="H22" s="3">
+        <v>0</v>
+      </c>
+      <c r="I22" s="4">
+        <v>9</v>
+      </c>
+      <c r="J22" s="4">
+        <v>2</v>
+      </c>
+      <c r="K22" s="4">
+        <v>6</v>
+      </c>
+      <c r="L22" s="4">
+        <v>2</v>
+      </c>
+      <c r="M22" s="5">
+        <v>3</v>
+      </c>
+      <c r="N22" s="5">
+        <v>2</v>
+      </c>
+      <c r="O22" s="5">
+        <v>2</v>
+      </c>
+      <c r="P22" s="5">
+        <v>3</v>
+      </c>
+      <c r="Q22" s="3">
+        <v>1</v>
+      </c>
+      <c r="R22" s="4">
+        <v>2</v>
+      </c>
+      <c r="S22" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="4:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D23" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E23" s="3">
+        <v>6</v>
+      </c>
+      <c r="F23" s="3">
+        <v>1</v>
+      </c>
+      <c r="G23" s="3">
+        <v>1</v>
+      </c>
+      <c r="H23" s="3">
+        <v>0</v>
+      </c>
+      <c r="I23" s="4">
+        <v>7</v>
+      </c>
+      <c r="J23" s="4">
+        <v>1</v>
+      </c>
+      <c r="K23" s="4">
+        <v>5</v>
+      </c>
+      <c r="L23" s="4">
+        <v>2</v>
+      </c>
+      <c r="M23" s="5">
+        <v>2</v>
+      </c>
+      <c r="N23" s="5">
+        <v>2</v>
+      </c>
+      <c r="O23" s="5">
+        <v>5</v>
+      </c>
+      <c r="P23" s="5">
+        <v>2</v>
+      </c>
+      <c r="Q23" s="3">
+        <v>0</v>
+      </c>
+      <c r="R23" s="4">
+        <v>1</v>
+      </c>
+      <c r="S23" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="4:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D24" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E24" s="3">
+        <v>3</v>
+      </c>
+      <c r="F24" s="3">
+        <v>2</v>
+      </c>
+      <c r="G24" s="3">
+        <v>1</v>
+      </c>
+      <c r="H24" s="3">
+        <v>1</v>
+      </c>
+      <c r="I24" s="5">
+        <v>4</v>
+      </c>
+      <c r="J24" s="5">
+        <v>3</v>
+      </c>
+      <c r="K24" s="3">
+        <v>0</v>
+      </c>
+      <c r="L24" s="3">
+        <v>0</v>
+      </c>
+      <c r="M24" s="3">
+        <v>1</v>
+      </c>
+      <c r="N24" s="3">
+        <v>1</v>
+      </c>
+      <c r="O24" s="5">
+        <v>2</v>
+      </c>
+      <c r="P24" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q24" s="3">
+        <v>0</v>
+      </c>
+      <c r="R24" s="4">
+        <v>1</v>
+      </c>
+      <c r="S24" s="3">
         <v>0</v>
       </c>
     </row>

</xml_diff>